<commit_message>
add feature to calculate credit cost and how many time you need to finish the stage, fix a display bug that the stage level is less than the actual one
</commit_message>
<xml_diff>
--- a/src/main/resources/character_upgrade.xlsx
+++ b/src/main/resources/character_upgrade.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Peronsal_project\StarRail_Calculator\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{235DDC45-B272-45B6-B5FF-FED2C0BAD8E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C200B86F-046F-46C9-8132-F0ABA115D4F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -368,7 +369,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C80"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
@@ -1338,4 +1339,116 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED0AD936-05DC-4A1B-87CF-9ACD86B65E7B}">
+  <dimension ref="A1:E6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1">
+        <f>0+D1</f>
+        <v>3200</v>
+      </c>
+      <c r="B1">
+        <f>0+E1</f>
+        <v>4000</v>
+      </c>
+      <c r="D1" s="1">
+        <v>3200</v>
+      </c>
+      <c r="E1" s="1">
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <f>A1+D2</f>
+        <v>9600</v>
+      </c>
+      <c r="B2">
+        <f>B1+E2</f>
+        <v>12000</v>
+      </c>
+      <c r="D2" s="1">
+        <v>6400</v>
+      </c>
+      <c r="E2" s="1">
+        <v>8000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <f t="shared" ref="A3:B6" si="0">A2+D3</f>
+        <v>22400</v>
+      </c>
+      <c r="B3">
+        <f t="shared" si="0"/>
+        <v>28000</v>
+      </c>
+      <c r="D3" s="1">
+        <v>12800</v>
+      </c>
+      <c r="E3" s="1">
+        <v>16000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <f t="shared" si="0"/>
+        <v>54400</v>
+      </c>
+      <c r="B4">
+        <f t="shared" si="0"/>
+        <v>68000</v>
+      </c>
+      <c r="D4" s="1">
+        <v>32000</v>
+      </c>
+      <c r="E4" s="1">
+        <v>40000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <f t="shared" si="0"/>
+        <v>118400</v>
+      </c>
+      <c r="B5">
+        <f t="shared" si="0"/>
+        <v>148000</v>
+      </c>
+      <c r="D5" s="1">
+        <v>64000</v>
+      </c>
+      <c r="E5" s="1">
+        <v>80000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <f t="shared" si="0"/>
+        <v>246400</v>
+      </c>
+      <c r="B6">
+        <f t="shared" si="0"/>
+        <v>308000</v>
+      </c>
+      <c r="D6" s="1">
+        <v>128000</v>
+      </c>
+      <c r="E6" s="1">
+        <v>160000</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>